<commit_message>
Change LOOCV_all_methods_plot() to grouped bar chart instead of stacked bar chart
</commit_message>
<xml_diff>
--- a/all_methods_LOOCV.xlsx
+++ b/all_methods_LOOCV.xlsx
@@ -1794,10 +1794,10 @@
         <v>1</v>
       </c>
       <c r="C93">
-        <v>1.842334896364348</v>
+        <v>1.726520939097383</v>
       </c>
       <c r="D93">
-        <v>0.5439107355084758</v>
+        <v>0.3851033057330708</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1808,10 +1808,10 @@
         <v>2</v>
       </c>
       <c r="C94">
-        <v>1.724176470651423</v>
+        <v>1.723815928865911</v>
       </c>
       <c r="D94">
-        <v>2.451890797651533</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1822,10 +1822,10 @@
         <v>3</v>
       </c>
       <c r="C95">
-        <v>1.764807718926551</v>
+        <v>1.726520939097383</v>
       </c>
       <c r="D95">
-        <v>1.975131214468673</v>
+        <v>1.476399494870698</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1836,10 +1836,10 @@
         <v>4</v>
       </c>
       <c r="C96">
-        <v>1.842334896364348</v>
+        <v>1.711907964432955</v>
       </c>
       <c r="D96">
-        <v>1.724176470651423</v>
+        <v>1.881861869792296</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1850,10 +1850,10 @@
         <v>5</v>
       </c>
       <c r="C97">
-        <v>1.88428030420445</v>
+        <v>1.863407532571061</v>
       </c>
       <c r="D97">
-        <v>1.48436268223967</v>
+        <v>0.9500000000000016</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1864,10 +1864,10 @@
         <v>6</v>
       </c>
       <c r="C98">
-        <v>1.919255165286654</v>
+        <v>1.881861869792296</v>
       </c>
       <c r="D98">
-        <v>1.705960871458994</v>
+        <v>1.517125022550414</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1878,10 +1878,10 @@
         <v>7</v>
       </c>
       <c r="C99">
-        <v>1.800389488524246</v>
+        <v>1.7</v>
       </c>
       <c r="D99">
-        <v>1.827690895346973</v>
+        <v>2.322552520830811</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1892,10 +1892,10 @@
         <v>8</v>
       </c>
       <c r="C100">
-        <v>1.800389488524246</v>
+        <v>1.729225949328855</v>
       </c>
       <c r="D100">
-        <v>1.631264734052657</v>
+        <v>1.38170376628553</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1906,10 +1906,10 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>1.901767734745552</v>
+        <v>1.796316740949958</v>
       </c>
       <c r="D101">
-        <v>1.06348959612772</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1920,10 +1920,10 @@
         <v>10</v>
       </c>
       <c r="C102">
-        <v>1.901767734745552</v>
+        <v>1.690930934896147</v>
       </c>
       <c r="D102">
-        <v>1.687355033525566</v>
+        <v>1.911658591101796</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1934,10 +1934,10 @@
         <v>11</v>
       </c>
       <c r="C103">
-        <v>1.729225949328855</v>
+        <v>1.723815928865911</v>
       </c>
       <c r="D103">
-        <v>2.088942737425522</v>
+        <v>1.612845903407933</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1948,10 +1948,10 @@
         <v>12</v>
       </c>
       <c r="C104">
-        <v>1.723996199758667</v>
+        <v>1.640930934896148</v>
       </c>
       <c r="D104">
-        <v>3.435699150537795</v>
+        <v>2.390949882737841</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1962,10 +1962,10 @@
         <v>13</v>
       </c>
       <c r="C105">
-        <v>1.764807718926551</v>
+        <v>1.7</v>
       </c>
       <c r="D105">
-        <v>2.72316382825862</v>
+        <v>2.800000000000002</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2158,10 +2158,10 @@
         <v>1</v>
       </c>
       <c r="C119">
-        <v>1.796435275425877</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D119">
-        <v>1.026475577390114</v>
+        <v>1.899999999999999</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2172,10 +2172,10 @@
         <v>2</v>
       </c>
       <c r="C120">
-        <v>1.779034956502331</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D120">
-        <v>2.199280035558578</v>
+        <v>2.149999999999999</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2186,10 +2186,10 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>1.763953940263578</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D121">
-        <v>2.348191508605357</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2200,10 +2200,10 @@
         <v>4</v>
       </c>
       <c r="C122">
-        <v>1.796435275425877</v>
+        <v>1.949999999999999</v>
       </c>
       <c r="D122">
-        <v>1.43257470964101</v>
+        <v>1.899999999999999</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2214,10 +2214,10 @@
         <v>5</v>
       </c>
       <c r="C123">
-        <v>1.797285016820926</v>
+        <v>1.9</v>
       </c>
       <c r="D123">
-        <v>1.495923691809002</v>
+        <v>0.9499999999999998</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2228,10 +2228,10 @@
         <v>6</v>
       </c>
       <c r="C124">
-        <v>1.748872924024825</v>
+        <v>2</v>
       </c>
       <c r="D124">
-        <v>1.956405597782479</v>
+        <v>1.449999999999998</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2242,10 +2242,10 @@
         <v>7</v>
       </c>
       <c r="C125">
-        <v>1.797285016820926</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D125">
-        <v>1.231096831219968</v>
+        <v>2.049999999999998</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2256,10 +2256,10 @@
         <v>8</v>
       </c>
       <c r="C126">
-        <v>1.795585534030828</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D126">
-        <v>1.406155959500823</v>
+        <v>2.100000000000002</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2270,10 +2270,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>1.839799034259984</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D127">
-        <v>1.130390356020555</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2284,10 +2284,10 @@
         <v>10</v>
       </c>
       <c r="C128">
-        <v>1.812492762560854</v>
+        <v>1.949999999999998</v>
       </c>
       <c r="D128">
-        <v>1.716801929012167</v>
+        <v>1.700000000000001</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2298,10 +2298,10 @@
         <v>11</v>
       </c>
       <c r="C129">
-        <v>1.795585534030828</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D129">
-        <v>1.79880414648426</v>
+        <v>2.225</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2312,10 +2312,10 @@
         <v>12</v>
       </c>
       <c r="C130">
-        <v>1.763953940263578</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D130">
-        <v>2.265911591168186</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2326,10 +2326,10 @@
         <v>13</v>
       </c>
       <c r="C131">
-        <v>1.787310245266579</v>
+        <v>1.750000000000002</v>
       </c>
       <c r="D131">
-        <v>2.075586377238414</v>
+        <v>3.599999999999996</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2522,10 +2522,10 @@
         <v>1</v>
       </c>
       <c r="C145">
-        <v>1.98790486489403</v>
+        <v>1.700000000000003</v>
       </c>
       <c r="D145">
-        <v>0.3477332271035962</v>
+        <v>0.3000000000000007</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2536,10 +2536,10 @@
         <v>2</v>
       </c>
       <c r="C146">
-        <v>1.900000000000004</v>
+        <v>1.699999999999999</v>
       </c>
       <c r="D146">
-        <v>2.45704429634281</v>
+        <v>2.150000000000001</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2550,10 +2550,10 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="D147">
-        <v>2.236355971587642</v>
+        <v>2.19999999999999</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2564,10 +2564,10 @@
         <v>4</v>
       </c>
       <c r="C148">
-        <v>2.043180996955727</v>
+        <v>1.7</v>
       </c>
       <c r="D148">
-        <v>1.900000000000004</v>
+        <v>1.899999999999999</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2578,10 +2578,10 @@
         <v>5</v>
       </c>
       <c r="C149">
-        <v>2.086361993911689</v>
+        <v>1.799999999999997</v>
       </c>
       <c r="D149">
-        <v>1.456818710399804</v>
+        <v>0.9500000000000007</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2592,10 +2592,10 @@
         <v>6</v>
       </c>
       <c r="C150">
-        <v>2.086361993911689</v>
+        <v>1.899999999999997</v>
       </c>
       <c r="D150">
-        <v>1.705409272097066</v>
+        <v>1.599999999999996</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2606,10 +2606,10 @@
         <v>7</v>
       </c>
       <c r="C151">
-        <v>1.975809729788294</v>
+        <v>1.699999999999999</v>
       </c>
       <c r="D151">
-        <v>1.916295326193516</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2620,10 +2620,10 @@
         <v>8</v>
       </c>
       <c r="C152">
-        <v>1.975809729788294</v>
+        <v>1.699999999999999</v>
       </c>
       <c r="D152">
-        <v>1.709402376145157</v>
+        <v>2.049999999999998</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2634,10 +2634,10 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>2.043180996955727</v>
+        <v>1.750000000000001</v>
       </c>
       <c r="D153">
-        <v>1.009092004058861</v>
+        <v>0.9999999999999982</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2648,10 +2648,10 @@
         <v>10</v>
       </c>
       <c r="C154">
-        <v>2.043180996955727</v>
+        <v>1.750000000000001</v>
       </c>
       <c r="D154">
-        <v>1.699931351231513</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2662,10 +2662,10 @@
         <v>11</v>
       </c>
       <c r="C155">
-        <v>1.975809729788294</v>
+        <v>1.700000000000005</v>
       </c>
       <c r="D155">
-        <v>2.22410700523707</v>
+        <v>1.599999999999998</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2676,10 +2676,10 @@
         <v>12</v>
       </c>
       <c r="C156">
-        <v>1.79633337362504</v>
+        <v>1.7</v>
       </c>
       <c r="D156">
-        <v>3.76816594114604</v>
+        <v>1.700000000000005</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2690,10 +2690,10 @@
         <v>13</v>
       </c>
       <c r="C157">
-        <v>1.9</v>
+        <v>1.674999999999997</v>
       </c>
       <c r="D157">
-        <v>2.815402524754566</v>
+        <v>2.800000000000001</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2886,10 +2886,10 @@
         <v>1</v>
       </c>
       <c r="C171">
-        <v>2.001921391493164</v>
+        <v>1.799854946004941</v>
       </c>
       <c r="D171">
-        <v>0.3198735611299135</v>
+        <v>0.3998241769756907</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2900,10 +2900,10 @@
         <v>2</v>
       </c>
       <c r="C172">
-        <v>1.901857887744856</v>
+        <v>1.70088312543526</v>
       </c>
       <c r="D172">
-        <v>2.453168188289558</v>
+        <v>2.095774087213929</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2914,10 +2914,10 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>1.899546101209396</v>
+        <v>1.704303480745202</v>
       </c>
       <c r="D173">
-        <v>2.273501926075422</v>
+        <v>2.599335395253127</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2928,10 +2928,10 @@
         <v>4</v>
       </c>
       <c r="C174">
-        <v>2.032750649626724</v>
+        <v>1.848582587146902</v>
       </c>
       <c r="D174">
-        <v>1.901857887744856</v>
+        <v>1.299999701387888</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2942,10 +2942,10 @@
         <v>5</v>
       </c>
       <c r="C175">
-        <v>2.012505151405017</v>
+        <v>1.799930859619868</v>
       </c>
       <c r="D175">
-        <v>1.452839070714683</v>
+        <v>0.949653170821309</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -2956,10 +2956,10 @@
         <v>6</v>
       </c>
       <c r="C176">
-        <v>2.052996147848432</v>
+        <v>1.799850550429333</v>
       </c>
       <c r="D176">
-        <v>1.702216642889907</v>
+        <v>2.000699106508631</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -2970,10 +2970,10 @@
         <v>7</v>
       </c>
       <c r="C177">
-        <v>1.991337631581312</v>
+        <v>1.707723836055143</v>
       </c>
       <c r="D177">
-        <v>1.930027638492524</v>
+        <v>1.849929661583651</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -2984,10 +2984,10 @@
         <v>8</v>
       </c>
       <c r="C178">
-        <v>1.991337631581312</v>
+        <v>1.70088312543526</v>
       </c>
       <c r="D178">
-        <v>1.718676294410953</v>
+        <v>2.899550116676336</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -2998,10 +2998,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>2.032750649626724</v>
+        <v>1.799895100600208</v>
       </c>
       <c r="D179">
-        <v>1.003811614450273</v>
+        <v>1.000026468030084</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3012,10 +3012,10 @@
         <v>10</v>
       </c>
       <c r="C180">
-        <v>2.032750649626724</v>
+        <v>1.799854946004941</v>
       </c>
       <c r="D180">
-        <v>1.699995269735226</v>
+        <v>1.698204311614964</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -3026,10 +3026,10 @@
         <v>11</v>
       </c>
       <c r="C181">
-        <v>1.991337631581312</v>
+        <v>1.799850550429333</v>
       </c>
       <c r="D181">
-        <v>2.23558488260412</v>
+        <v>1.598791128843338</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -3040,10 +3040,10 @@
         <v>12</v>
       </c>
       <c r="C182">
-        <v>1.799985123329988</v>
+        <v>1.799854946004941</v>
       </c>
       <c r="D182">
-        <v>3.430112160587614</v>
+        <v>1.70088312543526</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -3054,10 +3054,10 @@
         <v>13</v>
       </c>
       <c r="C183">
-        <v>1.899546101209396</v>
+        <v>1.704303480745202</v>
       </c>
       <c r="D183">
-        <v>2.802743482986237</v>
+        <v>2.298517724533779</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3250,10 +3250,10 @@
         <v>1</v>
       </c>
       <c r="C197">
-        <v>1.866258789215016</v>
+        <v>1.8</v>
       </c>
       <c r="D197">
-        <v>1.212608610658844</v>
+        <v>0.4000000000000008</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3264,10 +3264,10 @@
         <v>2</v>
       </c>
       <c r="C198">
-        <v>1.827626180445057</v>
+        <v>1.700000000000001</v>
       </c>
       <c r="D198">
-        <v>2.271687073507625</v>
+        <v>2.100000000000002</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3278,10 +3278,10 @@
         <v>3</v>
       </c>
       <c r="C199">
-        <v>1.842496927148795</v>
+        <v>1.700000000000002</v>
       </c>
       <c r="D199">
-        <v>2.61594602422289</v>
+        <v>2.600000000000001</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3292,10 +3292,10 @@
         <v>4</v>
       </c>
       <c r="C200">
-        <v>1.888492482756323</v>
+        <v>1.850000000000001</v>
       </c>
       <c r="D200">
-        <v>1.661101665808411</v>
+        <v>1.300000000000002</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3306,10 +3306,10 @@
         <v>5</v>
       </c>
       <c r="C201">
-        <v>1.868460047995983</v>
+        <v>1.800000000000002</v>
       </c>
       <c r="D201">
-        <v>1.43087091631382</v>
+        <v>0.9499999999999998</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3320,10 +3320,10 @@
         <v>6</v>
       </c>
       <c r="C202">
-        <v>1.831539952004015</v>
+        <v>1.799999999999999</v>
       </c>
       <c r="D202">
-        <v>2.421070414747719</v>
+        <v>1.999999999999999</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3334,10 +3334,10 @@
         <v>7</v>
       </c>
       <c r="C203">
-        <v>1.864057530434048</v>
+        <v>1.700000000000002</v>
       </c>
       <c r="D203">
-        <v>1.65692106928871</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3348,10 +3348,10 @@
         <v>8</v>
       </c>
       <c r="C204">
-        <v>1.864057530434048</v>
+        <v>1.700000000000001</v>
       </c>
       <c r="D204">
-        <v>1.356443624795877</v>
+        <v>2.899999999999999</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3362,10 +3362,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>1.888492482756323</v>
+        <v>1.800000000000002</v>
       </c>
       <c r="D205">
-        <v>1.154359968002677</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3376,10 +3376,10 @@
         <v>10</v>
       </c>
       <c r="C206">
-        <v>1.858755716363812</v>
+        <v>1.8</v>
       </c>
       <c r="D206">
-        <v>1.876984965512647</v>
+        <v>1.700000000000002</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3390,10 +3390,10 @@
         <v>11</v>
       </c>
       <c r="C207">
-        <v>1.868460047995983</v>
+        <v>1.799999999999999</v>
       </c>
       <c r="D207">
-        <v>1.730801272673144</v>
+        <v>1.599999999999999</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3404,10 +3404,10 @@
         <v>12</v>
       </c>
       <c r="C208">
-        <v>1.866258789215016</v>
+        <v>1.8</v>
       </c>
       <c r="D208">
-        <v>1.661780463961172</v>
+        <v>1.699999999999999</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3418,10 +3418,10 @@
         <v>13</v>
       </c>
       <c r="C209">
-        <v>1.842496927148795</v>
+        <v>1.700000000000002</v>
       </c>
       <c r="D209">
-        <v>2.021994389114123</v>
+        <v>2.299999999999999</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3614,10 +3614,10 @@
         <v>1</v>
       </c>
       <c r="C223">
-        <v>1.759794991844502</v>
+        <v>1.799999999999995</v>
       </c>
       <c r="D223">
-        <v>0.9160060861504391</v>
+        <v>0.3999999999999995</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3628,10 +3628,10 @@
         <v>2</v>
       </c>
       <c r="C224">
-        <v>1.743393796891427</v>
+        <v>1.700000000000003</v>
       </c>
       <c r="D224">
-        <v>2.244432831058005</v>
+        <v>2.099999999999999</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3642,10 +3642,10 @@
         <v>3</v>
       </c>
       <c r="C225">
-        <v>1.733417590431569</v>
+        <v>1.700000000000009</v>
       </c>
       <c r="D225">
-        <v>2.200000000000002</v>
+        <v>2.600000000000001</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3656,10 +3656,10 @@
         <v>4</v>
       </c>
       <c r="C226">
-        <v>1.763053130155554</v>
+        <v>1.849999999999999</v>
       </c>
       <c r="D226">
-        <v>1.213855217815125</v>
+        <v>1.300000000000004</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3670,10 +3670,10 @@
         <v>5</v>
       </c>
       <c r="C227">
-        <v>1.755885469710477</v>
+        <v>1.799999999999999</v>
       </c>
       <c r="D227">
-        <v>1.511093811018953</v>
+        <v>0.9500000000000004</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3684,10 +3684,10 @@
         <v>6</v>
       </c>
       <c r="C228">
-        <v>1.755885469710477</v>
+        <v>1.799999999999991</v>
       </c>
       <c r="D228">
-        <v>1.747211026766009</v>
+        <v>2.00000000000001</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3698,10 +3698,10 @@
         <v>7</v>
       </c>
       <c r="C229">
-        <v>1.763704513978528</v>
+        <v>1.700000000000014</v>
       </c>
       <c r="D229">
-        <v>1.649254600076436</v>
+        <v>1.849999999999999</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3712,10 +3712,10 @@
         <v>8</v>
       </c>
       <c r="C230">
-        <v>1.755885469710477</v>
+        <v>1.700000000000003</v>
       </c>
       <c r="D230">
-        <v>1.415024160917953</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3726,10 +3726,10 @@
         <v>9</v>
       </c>
       <c r="C231">
-        <v>1.76696265228958</v>
+        <v>1.799999999999999</v>
       </c>
       <c r="D231">
-        <v>1.113480527067088</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3740,10 +3740,10 @@
         <v>10</v>
       </c>
       <c r="C232">
-        <v>1.76696265228958</v>
+        <v>1.799999999999995</v>
       </c>
       <c r="D232">
-        <v>1.639445083548781</v>
+        <v>1.699999999999999</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3754,10 +3754,10 @@
         <v>11</v>
       </c>
       <c r="C233">
-        <v>1.755885469710477</v>
+        <v>1.799999999999991</v>
       </c>
       <c r="D233">
-        <v>1.847993535722271</v>
+        <v>1.599999999999999</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3768,10 +3768,10 @@
         <v>12</v>
       </c>
       <c r="C234">
-        <v>1.711720691985857</v>
+        <v>1.799999999999995</v>
       </c>
       <c r="D234">
-        <v>2.900000000000005</v>
+        <v>1.699999999999998</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3782,10 +3782,10 @@
         <v>13</v>
       </c>
       <c r="C235">
-        <v>1.753549155434977</v>
+        <v>1.700000000000009</v>
       </c>
       <c r="D235">
-        <v>1.755885469710477</v>
+        <v>2.300000000000002</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3950,7 +3950,7 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>2.300000000001484</v>
+        <v>2.256044028832367</v>
       </c>
       <c r="D247">
         <v>1.244063558990144</v>
@@ -3964,7 +3964,7 @@
         <v>2</v>
       </c>
       <c r="C248">
-        <v>2.269265937668471</v>
+        <v>2.155578789463637</v>
       </c>
       <c r="D248">
         <v>2.399985494719896</v>
@@ -3978,7 +3978,7 @@
         <v>3</v>
       </c>
       <c r="C249">
-        <v>2.282487848455621</v>
+        <v>2.167345412628075</v>
       </c>
       <c r="D249">
         <v>2.491249024802263</v>
@@ -3992,7 +3992,7 @@
         <v>4</v>
       </c>
       <c r="C250">
-        <v>2.282487848455621</v>
+        <v>2.182498049600692</v>
       </c>
       <c r="D250">
         <v>2.357916832628158</v>
@@ -4006,10 +4006,10 @@
         <v>5</v>
       </c>
       <c r="C251">
-        <v>2.269265937668471</v>
+        <v>2.21927103921653</v>
       </c>
       <c r="D251">
-        <v>2.300000000001484</v>
+        <v>1.722890026030939</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -4020,7 +4020,7 @@
         <v>6</v>
       </c>
       <c r="C252">
-        <v>2.278022013441402</v>
+        <v>2.174921731114384</v>
       </c>
       <c r="D252">
         <v>2.282487848455621</v>
@@ -4034,10 +4034,10 @@
         <v>7</v>
       </c>
       <c r="C253">
-        <v>2.291243924228552</v>
+        <v>2.21927103921653</v>
       </c>
       <c r="D253">
-        <v>2.074821010628762</v>
+        <v>1.500764687149843</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -4048,10 +4048,10 @@
         <v>8</v>
       </c>
       <c r="C254">
-        <v>2.374511022242315</v>
+        <v>2.291243924228581</v>
       </c>
       <c r="D254">
-        <v>1.613630043460906</v>
+        <v>1.527252641287578</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -4062,7 +4062,7 @@
         <v>9</v>
       </c>
       <c r="C255">
-        <v>2.269265937668471</v>
+        <v>2.174921731114384</v>
       </c>
       <c r="D255">
         <v>2.798465390281888</v>
@@ -4076,10 +4076,10 @@
         <v>10</v>
       </c>
       <c r="C256">
-        <v>2.182498049600692</v>
+        <v>2.148002470977328</v>
       </c>
       <c r="D256">
-        <v>3.840422524506292</v>
+        <v>3.410189132488982</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -4090,10 +4090,10 @@
         <v>11</v>
       </c>
       <c r="C257">
-        <v>2.282487848455621</v>
+        <v>2.167345412628075</v>
       </c>
       <c r="D257">
-        <v>2.330775029906937</v>
+        <v>2.330774980730596</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -4258,7 +4258,7 @@
         <v>1</v>
       </c>
       <c r="C269">
-        <v>2.277342983882734</v>
+        <v>2.318942133651886</v>
       </c>
       <c r="D269">
         <v>1.611982263375424</v>
@@ -4272,7 +4272,7 @@
         <v>2</v>
       </c>
       <c r="C270">
-        <v>2.130553504621597</v>
+        <v>2.190790826381308</v>
       </c>
       <c r="D270">
         <v>2.370763978183541</v>
@@ -4286,7 +4286,7 @@
         <v>3</v>
       </c>
       <c r="C271">
-        <v>2.231610143743993</v>
+        <v>2.277342983882734</v>
       </c>
       <c r="D271">
         <v>2.67850991758823</v>
@@ -4300,7 +4300,7 @@
         <v>4</v>
       </c>
       <c r="C272">
-        <v>2.28854302530376</v>
+        <v>2.393898427392598</v>
       </c>
       <c r="D272">
         <v>1.857282414116367</v>
@@ -4314,10 +4314,10 @@
         <v>5</v>
       </c>
       <c r="C273">
-        <v>2.245527413434496</v>
+        <v>2.289258056268273</v>
       </c>
       <c r="D273">
-        <v>2.390394406334826</v>
+        <v>2.393898427392598</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4328,7 +4328,7 @@
         <v>6</v>
       </c>
       <c r="C274">
-        <v>2.245527413434496</v>
+        <v>2.289258056268273</v>
       </c>
       <c r="D274">
         <v>2.799999999999998</v>
@@ -4342,10 +4342,10 @@
         <v>7</v>
       </c>
       <c r="C275">
-        <v>2.294858076978786</v>
+        <v>2.344853055917714</v>
       </c>
       <c r="D275">
-        <v>1.247541680578767</v>
+        <v>0.399999999999995</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4356,10 +4356,10 @@
         <v>8</v>
       </c>
       <c r="C276">
-        <v>2.277342983882734</v>
+        <v>2.344853055917714</v>
       </c>
       <c r="D276">
-        <v>1.710749825221872</v>
+        <v>1.444945235178989</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -4370,7 +4370,7 @@
         <v>9</v>
       </c>
       <c r="C277">
-        <v>2.245527413434496</v>
+        <v>2.289258056268273</v>
       </c>
       <c r="D277">
         <v>2.607640627844465</v>
@@ -4384,10 +4384,10 @@
         <v>10</v>
       </c>
       <c r="C278">
-        <v>2.157609398562472</v>
+        <v>2.190790826381308</v>
       </c>
       <c r="D278">
-        <v>3.071294633375678</v>
+        <v>4.400000000000013</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4398,10 +4398,10 @@
         <v>11</v>
       </c>
       <c r="C279">
-        <v>2.277342983882734</v>
+        <v>2.301173128653812</v>
       </c>
       <c r="D279">
-        <v>2.208527040843736</v>
+        <v>2.392923053858372</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -4566,7 +4566,7 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>2.277342983882729</v>
+        <v>2.3189421336519</v>
       </c>
       <c r="D291">
         <v>1.611982263375425</v>
@@ -4580,7 +4580,7 @@
         <v>2</v>
       </c>
       <c r="C292">
-        <v>2.194609771153235</v>
+        <v>2.190790826381319</v>
       </c>
       <c r="D292">
         <v>2.370763978183534</v>
@@ -4594,7 +4594,7 @@
         <v>3</v>
       </c>
       <c r="C293">
-        <v>2.259444683124977</v>
+        <v>2.277342983882729</v>
       </c>
       <c r="D293">
         <v>2.678509917588267</v>
@@ -4608,7 +4608,7 @@
         <v>4</v>
       </c>
       <c r="C294">
-        <v>2.288543025304055</v>
+        <v>2.393898427392566</v>
       </c>
       <c r="D294">
         <v>1.857282414116358</v>
@@ -4622,10 +4622,10 @@
         <v>5</v>
       </c>
       <c r="C295">
-        <v>2.26502323731182</v>
+        <v>2.289258056268269</v>
       </c>
       <c r="D295">
-        <v>2.390394406334837</v>
+        <v>2.393898427392566</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -4636,7 +4636,7 @@
         <v>6</v>
       </c>
       <c r="C296">
-        <v>2.26502323731182</v>
+        <v>2.289258056268269</v>
       </c>
       <c r="D296">
         <v>2.800000000000003</v>
@@ -4650,10 +4650,10 @@
         <v>7</v>
       </c>
       <c r="C297">
-        <v>2.294858076978932</v>
+        <v>2.344853055917717</v>
       </c>
       <c r="D297">
-        <v>1.247541680578788</v>
+        <v>0.3999999999999666</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -4664,10 +4664,10 @@
         <v>8</v>
       </c>
       <c r="C298">
-        <v>2.277342983882729</v>
+        <v>2.344853055917717</v>
       </c>
       <c r="D298">
-        <v>1.710749825221931</v>
+        <v>1.444945235179145</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -4678,7 +4678,7 @@
         <v>9</v>
       </c>
       <c r="C299">
-        <v>2.26502323731182</v>
+        <v>2.289258056268269</v>
       </c>
       <c r="D299">
         <v>2.607640627844476</v>
@@ -4692,10 +4692,10 @@
         <v>10</v>
       </c>
       <c r="C300">
-        <v>2.157609398562469</v>
+        <v>2.190790826381319</v>
       </c>
       <c r="D300">
-        <v>3.071294633375676</v>
+        <v>4.400000000000002</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -4706,10 +4706,10 @@
         <v>11</v>
       </c>
       <c r="C301">
-        <v>2.277342983882729</v>
+        <v>2.301173128653809</v>
       </c>
       <c r="D301">
-        <v>2.208527040843723</v>
+        <v>2.392923053858396</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -4874,10 +4874,10 @@
         <v>1</v>
       </c>
       <c r="C313">
-        <v>2.300000000013734</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="D313">
-        <v>1.255717449062197</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -4888,10 +4888,10 @@
         <v>2</v>
       </c>
       <c r="C314">
-        <v>2.239033030779925</v>
+        <v>2.250253528172243</v>
       </c>
       <c r="D314">
-        <v>2.536690949158039</v>
+        <v>2.399999999999999</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -4902,10 +4902,10 @@
         <v>3</v>
       </c>
       <c r="C315">
-        <v>2.252794801079151</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="D315">
-        <v>2.475711313243475</v>
+        <v>2.156153699211791</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -4916,10 +4916,10 @@
         <v>4</v>
       </c>
       <c r="C316">
-        <v>2.252794801079151</v>
+        <v>2.1</v>
       </c>
       <c r="D316">
-        <v>2.376213184987177</v>
+        <v>4.054861140340476</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -4930,10 +4930,10 @@
         <v>5</v>
       </c>
       <c r="C317">
-        <v>2.252096372379159</v>
+        <v>2.250253528172243</v>
       </c>
       <c r="D317">
-        <v>2.300000000013734</v>
+        <v>2.300000000000001</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -4944,10 +4944,10 @@
         <v>6</v>
       </c>
       <c r="C318">
-        <v>2.276397400546442</v>
+        <v>2.3</v>
       </c>
       <c r="D318">
-        <v>2.251397943679167</v>
+        <v>1.856523089996617</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -4958,10 +4958,10 @@
         <v>7</v>
       </c>
       <c r="C319">
-        <v>2.276397400546442</v>
+        <v>2.399999999999999</v>
       </c>
       <c r="D319">
-        <v>2.068161991382249</v>
+        <v>0.4832841254210782</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -4972,10 +4972,10 @@
         <v>8</v>
       </c>
       <c r="C320">
-        <v>2.383419547829869</v>
+        <v>2.399999999999999</v>
       </c>
       <c r="D320">
-        <v>1.606021398301308</v>
+        <v>1.300000000000002</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -4986,10 +4986,10 @@
         <v>9</v>
       </c>
       <c r="C321">
-        <v>2.252096372379159</v>
+        <v>2.200253528172244</v>
       </c>
       <c r="D321">
-        <v>2.797204848811806</v>
+        <v>2.886935181166583</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -5000,10 +5000,10 @@
         <v>10</v>
       </c>
       <c r="C322">
-        <v>2.226668117880683</v>
+        <v>2.3</v>
       </c>
       <c r="D322">
-        <v>3.823460698236347</v>
+        <v>1.350784139260229</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -5014,10 +5014,10 @@
         <v>11</v>
       </c>
       <c r="C323">
-        <v>2.300000000013734</v>
+        <v>2.200000000000001</v>
       </c>
       <c r="D323">
-        <v>2.239731459479917</v>
+        <v>3.63954954508331</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -5182,10 +5182,10 @@
         <v>1</v>
       </c>
       <c r="C335">
-        <v>2.287966725515082</v>
+        <v>3.4</v>
       </c>
       <c r="D335">
-        <v>1.482262170349453</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -5196,10 +5196,10 @@
         <v>2</v>
       </c>
       <c r="C336">
-        <v>2.120499842886067</v>
+        <v>2.9</v>
       </c>
       <c r="D336">
-        <v>2.340585820798213</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -5210,10 +5210,10 @@
         <v>3</v>
       </c>
       <c r="C337">
-        <v>2.178823618581944</v>
+        <v>3.4</v>
       </c>
       <c r="D337">
-        <v>2.436807378192086</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -5224,10 +5224,10 @@
         <v>4</v>
       </c>
       <c r="C338">
-        <v>2.287966725515082</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="D338">
-        <v>1.920186069097177</v>
+        <v>4.499999999999995</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -5238,10 +5238,10 @@
         <v>5</v>
       </c>
       <c r="C339">
-        <v>2.120499842886067</v>
+        <v>3.399999999999999</v>
       </c>
       <c r="D339">
-        <v>2.30054056055083</v>
+        <v>3</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5252,10 +5252,10 @@
         <v>6</v>
       </c>
       <c r="C340">
-        <v>2.233395172048513</v>
+        <v>3.649999999999987</v>
       </c>
       <c r="D340">
-        <v>1.648443771605781</v>
+        <v>1.474999999999996</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5266,10 +5266,10 @@
         <v>7</v>
       </c>
       <c r="C341">
-        <v>2.294253643032956</v>
+        <v>3.500000000000002</v>
       </c>
       <c r="D341">
-        <v>1.458368614304646</v>
+        <v>1.900000000000009</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5280,10 +5280,10 @@
         <v>8</v>
       </c>
       <c r="C342">
-        <v>2.287966725515082</v>
+        <v>3.500000000000002</v>
       </c>
       <c r="D342">
-        <v>1.717528605698827</v>
+        <v>2.200000000000005</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -5294,10 +5294,10 @@
         <v>9</v>
       </c>
       <c r="C343">
-        <v>2.15959787838815</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="D343">
-        <v>2.717856653034997</v>
+        <v>4.300000000000003</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -5308,10 +5308,10 @@
         <v>10</v>
       </c>
       <c r="C344">
-        <v>2.073651754848882</v>
+        <v>2.800000000000001</v>
       </c>
       <c r="D344">
-        <v>4.560926962780122</v>
+        <v>5.900000000000006</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -5322,10 +5322,10 @@
         <v>11</v>
       </c>
       <c r="C345">
-        <v>2.287966725515082</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="D345">
-        <v>2.011549725355799</v>
+        <v>4.000000000000001</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -5490,10 +5490,10 @@
         <v>1</v>
       </c>
       <c r="C357">
-        <v>2.399999996187898</v>
+        <v>2.8</v>
       </c>
       <c r="D357">
-        <v>1.208979529901459</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -5504,10 +5504,10 @@
         <v>2</v>
       </c>
       <c r="C358">
-        <v>2.288027293907118</v>
+        <v>2.75</v>
       </c>
       <c r="D358">
-        <v>2.505984594022395</v>
+        <v>4.999999999999997</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -5518,10 +5518,10 @@
         <v>3</v>
       </c>
       <c r="C359">
-        <v>2.376054587814123</v>
+        <v>2.8</v>
       </c>
       <c r="D359">
-        <v>2.538027293907063</v>
+        <v>2.549999999999999</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -5532,10 +5532,10 @@
         <v>4</v>
       </c>
       <c r="C360">
-        <v>2.376054587814123</v>
+        <v>2.799999999999999</v>
       </c>
       <c r="D360">
-        <v>2.310258808849567</v>
+        <v>4.500000000000581</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -5546,10 +5546,10 @@
         <v>5</v>
       </c>
       <c r="C361">
-        <v>2.326054587814119</v>
+        <v>2.799999999999999</v>
       </c>
       <c r="D361">
-        <v>2.800855193281807</v>
+        <v>2.799999999999999</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -5560,10 +5560,10 @@
         <v>6</v>
       </c>
       <c r="C362">
-        <v>2.349999998094009</v>
+        <v>2.800000000000001</v>
       </c>
       <c r="D362">
-        <v>2.376054587814123</v>
+        <v>1.924999999999986</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -5574,10 +5574,10 @@
         <v>7</v>
       </c>
       <c r="C363">
-        <v>2.452992295105147</v>
+        <v>2.800000000000001</v>
       </c>
       <c r="D363">
-        <v>1.500028661817229</v>
+        <v>1.899999999977911</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -5588,10 +5588,10 @@
         <v>8</v>
       </c>
       <c r="C364">
-        <v>2.399999996187898</v>
+        <v>2.800000000000001</v>
       </c>
       <c r="D364">
-        <v>1.942730857014097</v>
+        <v>1.699999999999999</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -5602,10 +5602,10 @@
         <v>9</v>
       </c>
       <c r="C365">
-        <v>2.338027293907122</v>
+        <v>2.75</v>
       </c>
       <c r="D365">
-        <v>2.799981116978199</v>
+        <v>3.100000000000113</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -5616,10 +5616,10 @@
         <v>10</v>
       </c>
       <c r="C366">
-        <v>2.276054587814116</v>
+        <v>2.650000000007466</v>
       </c>
       <c r="D366">
-        <v>3.888491689838438</v>
+        <v>5.599999999987723</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -5630,10 +5630,10 @@
         <v>11</v>
       </c>
       <c r="C367">
-        <v>2.399999996187898</v>
+        <v>2.700000000000001</v>
       </c>
       <c r="D367">
-        <v>2.161598654463815</v>
+        <v>4.000000000031983</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -5798,10 +5798,10 @@
         <v>1</v>
       </c>
       <c r="C379">
-        <v>2.282757153165893</v>
+        <v>1.951326476249987</v>
       </c>
       <c r="D379">
-        <v>1.643762080011425</v>
+        <v>1.219198198456737</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -5812,10 +5812,10 @@
         <v>2</v>
       </c>
       <c r="C380">
-        <v>2.249601243208005</v>
+        <v>1.995615656838568</v>
       </c>
       <c r="D380">
-        <v>2.391469144150186</v>
+        <v>1.795734222506175</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -5826,10 +5826,10 @@
         <v>3</v>
       </c>
       <c r="C381">
-        <v>2.233811553333489</v>
+        <v>1.920882962377887</v>
       </c>
       <c r="D381">
-        <v>2.833281161072219</v>
+        <v>2.336868529639339</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -5840,10 +5840,10 @@
         <v>4</v>
       </c>
       <c r="C382">
-        <v>2.385314904566443</v>
+        <v>1.992623994293925</v>
       </c>
       <c r="D382">
-        <v>1.862409703543808</v>
+        <v>1.413737330958472</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -5854,10 +5854,10 @@
         <v>5</v>
       </c>
       <c r="C383">
-        <v>2.185907511674455</v>
+        <v>1.936104719313937</v>
       </c>
       <c r="D383">
-        <v>2.614586018101109</v>
+        <v>2.125572093915082</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -5868,10 +5868,10 @@
         <v>6</v>
       </c>
       <c r="C384">
-        <v>2.249601243208005</v>
+        <v>1.971975235271956</v>
       </c>
       <c r="D384">
-        <v>2.836395876637724</v>
+        <v>1.920882962377887</v>
       </c>
     </row>
     <row r="385" spans="1:4">
@@ -5882,10 +5882,10 @@
         <v>7</v>
       </c>
       <c r="C385">
-        <v>2.274074043124207</v>
+        <v>1.858308592442031</v>
       </c>
       <c r="D385">
-        <v>1.860761179495114</v>
+        <v>3.509652866259966</v>
       </c>
     </row>
     <row r="386" spans="1:4">
@@ -5896,10 +5896,10 @@
         <v>8</v>
       </c>
       <c r="C386">
-        <v>2.310300193216545</v>
+        <v>1.971975235271956</v>
       </c>
       <c r="D386">
-        <v>1.920456885504793</v>
+        <v>1.536470744074909</v>
       </c>
     </row>
     <row r="387" spans="1:4">
@@ -5910,10 +5910,10 @@
         <v>9</v>
       </c>
       <c r="C387">
-        <v>2.249601243208005</v>
+        <v>1.936104719313937</v>
       </c>
       <c r="D387">
-        <v>2.385314904566443</v>
+        <v>2.524327379067826</v>
       </c>
     </row>
     <row r="388" spans="1:4">
@@ -5924,10 +5924,10 @@
         <v>10</v>
       </c>
       <c r="C388">
-        <v>2.20956576073887</v>
+        <v>1.971975235271956</v>
       </c>
       <c r="D388">
-        <v>2.960720203745012</v>
+        <v>1.009356559346381</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -5938,10 +5938,10 @@
         <v>11</v>
       </c>
       <c r="C389">
-        <v>2.265390933082521</v>
+        <v>1.951326476249987</v>
       </c>
       <c r="D389">
-        <v>2.189912995147368</v>
+        <v>1.951437928445946</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -6106,10 +6106,10 @@
         <v>1</v>
       </c>
       <c r="C401">
-        <v>2.301230731047001</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="D401">
-        <v>1.499368720033806</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="402" spans="1:4">
@@ -6120,10 +6120,10 @@
         <v>2</v>
       </c>
       <c r="C402">
-        <v>2.119560555100557</v>
+        <v>1.950000000000002</v>
       </c>
       <c r="D402">
-        <v>2.331621042166264</v>
+        <v>1.800000000000009</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -6134,10 +6134,10 @@
         <v>3</v>
       </c>
       <c r="C403">
-        <v>2.241746531647912</v>
+        <v>1.800000000000009</v>
       </c>
       <c r="D403">
-        <v>2.469120399446002</v>
+        <v>2.500000000000004</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -6148,10 +6148,10 @@
         <v>4</v>
       </c>
       <c r="C404">
-        <v>2.301230731047001</v>
+        <v>2.000000000000016</v>
       </c>
       <c r="D404">
-        <v>1.712669690560452</v>
+        <v>1.400000000000007</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -6162,10 +6162,10 @@
         <v>5</v>
       </c>
       <c r="C405">
-        <v>2.156764233170415</v>
+        <v>1.950000000000002</v>
       </c>
       <c r="D405">
-        <v>2.301230731047001</v>
+        <v>1.700000000000004</v>
       </c>
     </row>
     <row r="406" spans="1:4">
@@ -6176,10 +6176,10 @@
         <v>6</v>
       </c>
       <c r="C406">
-        <v>2.271488631347457</v>
+        <v>1.900000000000007</v>
       </c>
       <c r="D406">
-        <v>1.620429426772873</v>
+        <v>1.899999999999999</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -6190,10 +6190,10 @@
         <v>7</v>
       </c>
       <c r="C407">
-        <v>2.310967605385159</v>
+        <v>1.800000000000004</v>
       </c>
       <c r="D407">
-        <v>1.442831496513303</v>
+        <v>3.699999999999996</v>
       </c>
     </row>
     <row r="408" spans="1:4">
@@ -6204,10 +6204,10 @@
         <v>8</v>
       </c>
       <c r="C408">
-        <v>2.301230731047001</v>
+        <v>1.950000000000002</v>
       </c>
       <c r="D408">
-        <v>1.701221456382485</v>
+        <v>1.699999999999999</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -6218,10 +6218,10 @@
         <v>9</v>
       </c>
       <c r="C409">
-        <v>2.20848275855692</v>
+        <v>1.850000000000004</v>
       </c>
       <c r="D409">
-        <v>2.706365116272191</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -6232,10 +6232,10 @@
         <v>10</v>
       </c>
       <c r="C410">
-        <v>2.100811629326213</v>
+        <v>2.000000000000011</v>
       </c>
       <c r="D410">
-        <v>3.491239045140354</v>
+        <v>0.8000000000000007</v>
       </c>
     </row>
     <row r="411" spans="1:4">
@@ -6246,10 +6246,10 @@
         <v>11</v>
       </c>
       <c r="C411">
-        <v>2.301230731047001</v>
+        <v>1.8</v>
       </c>
       <c r="D411">
-        <v>1.993002426932445</v>
+        <v>2.550000000000001</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -6414,10 +6414,10 @@
         <v>1</v>
       </c>
       <c r="C423">
-        <v>2.399999450263191</v>
+        <v>1.900000000000004</v>
       </c>
       <c r="D423">
-        <v>1.223589838781731</v>
+        <v>1.200000000000007</v>
       </c>
     </row>
     <row r="424" spans="1:4">
@@ -6428,10 +6428,10 @@
         <v>2</v>
       </c>
       <c r="C424">
-        <v>2.280628304568405</v>
+        <v>1.950000000000028</v>
       </c>
       <c r="D424">
-        <v>2.515693909194689</v>
+        <v>1.800000000000066</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -6442,10 +6442,10 @@
         <v>3</v>
       </c>
       <c r="C425">
-        <v>2.337093805030748</v>
+        <v>1.800000000000066</v>
       </c>
       <c r="D425">
-        <v>2.518546902515371</v>
+        <v>2.500000000000032</v>
       </c>
     </row>
     <row r="426" spans="1:4">
@@ -6456,10 +6456,10 @@
         <v>4</v>
       </c>
       <c r="C426">
-        <v>2.337093805030748</v>
+        <v>2.000000000000233</v>
       </c>
       <c r="D426">
-        <v>2.328346440763896</v>
+        <v>1.40000000000001</v>
       </c>
     </row>
     <row r="427" spans="1:4">
@@ -6470,10 +6470,10 @@
         <v>5</v>
       </c>
       <c r="C427">
-        <v>2.299175207083791</v>
+        <v>1.950000000000028</v>
       </c>
       <c r="D427">
-        <v>2.449090196451353</v>
+        <v>1.700000000000003</v>
       </c>
     </row>
     <row r="428" spans="1:4">
@@ -6484,10 +6484,10 @@
         <v>6</v>
       </c>
       <c r="C428">
-        <v>2.349999725131585</v>
+        <v>1.900000000000059</v>
       </c>
       <c r="D428">
-        <v>2.337093805030748</v>
+        <v>1.900000000000004</v>
       </c>
     </row>
     <row r="429" spans="1:4">
@@ -6498,10 +6498,10 @@
         <v>7</v>
       </c>
       <c r="C429">
-        <v>2.424544823357272</v>
+        <v>1.80000000000003</v>
       </c>
       <c r="D429">
-        <v>1.500190237014113</v>
+        <v>3.700000000000006</v>
       </c>
     </row>
     <row r="430" spans="1:4">
@@ -6512,10 +6512,10 @@
         <v>8</v>
       </c>
       <c r="C430">
-        <v>2.399999450263191</v>
+        <v>1.950000000000119</v>
       </c>
       <c r="D430">
-        <v>1.930903476207495</v>
+        <v>1.700000000000006</v>
       </c>
     </row>
     <row r="431" spans="1:4">
@@ -6526,10 +6526,10 @@
         <v>9</v>
       </c>
       <c r="C431">
-        <v>2.318546902515363</v>
+        <v>1.850000000000035</v>
       </c>
       <c r="D431">
-        <v>2.799747590048651</v>
+        <v>2.700000000000033</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -6540,10 +6540,10 @@
         <v>10</v>
       </c>
       <c r="C432">
-        <v>2.261256609136833</v>
+        <v>2.000000000000143</v>
       </c>
       <c r="D432">
-        <v>3.869926206375472</v>
+        <v>0.7999999999999936</v>
       </c>
     </row>
     <row r="433" spans="1:4">
@@ -6554,10 +6554,10 @@
         <v>11</v>
       </c>
       <c r="C433">
-        <v>2.399999450263191</v>
+        <v>1.799999999999995</v>
       </c>
       <c r="D433">
-        <v>2.153555013815968</v>
+        <v>2.550000000000011</v>
       </c>
     </row>
   </sheetData>
@@ -6666,10 +6666,10 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>1.800389488524246</v>
+        <v>1.723815928865911</v>
       </c>
       <c r="C9">
-        <v>1.724176470651423</v>
+        <v>1.612845903407933</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -6688,10 +6688,10 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1.795585534030828</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="C11">
-        <v>1.716801929012167</v>
+        <v>2.049999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -6710,10 +6710,10 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>1.975809729788294</v>
+        <v>1.7</v>
       </c>
       <c r="C13">
-        <v>1.900000000000004</v>
+        <v>1.700000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -6732,10 +6732,10 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>1.991337631581312</v>
+        <v>1.799850550429333</v>
       </c>
       <c r="C15">
-        <v>1.901857887744856</v>
+        <v>1.70088312543526</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -6754,10 +6754,10 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>1.864057530434048</v>
+        <v>1.799999999999999</v>
       </c>
       <c r="C17">
-        <v>1.661780463961172</v>
+        <v>1.700000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -6776,10 +6776,10 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>1.755885469710477</v>
+        <v>1.799999999999991</v>
       </c>
       <c r="C19">
-        <v>1.649254600076436</v>
+        <v>1.699999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -6798,10 +6798,10 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>2.282487848455621</v>
+        <v>2.174921731114384</v>
       </c>
       <c r="C21">
-        <v>2.330775029906937</v>
+        <v>2.330774980730596</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -6820,10 +6820,10 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>2.245527413434496</v>
+        <v>2.289258056268273</v>
       </c>
       <c r="C23">
-        <v>2.370763978183541</v>
+        <v>2.392923053858372</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -6842,10 +6842,10 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>2.26502323731182</v>
+        <v>2.289258056268269</v>
       </c>
       <c r="C25">
-        <v>2.370763978183534</v>
+        <v>2.392923053858396</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -6864,10 +6864,10 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>2.252794801079151</v>
+        <v>2.3</v>
       </c>
       <c r="C27">
-        <v>2.300000000013734</v>
+        <v>2.156153699211791</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -6886,10 +6886,10 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>2.233395172048513</v>
+        <v>3.399999999999999</v>
       </c>
       <c r="C29">
-        <v>2.011549725355799</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -6908,10 +6908,10 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>2.376054587814123</v>
+        <v>2.799999999999999</v>
       </c>
       <c r="C31">
-        <v>2.376054587814123</v>
+        <v>2.799999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -6930,10 +6930,10 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>2.249601243208005</v>
+        <v>1.951326476249987</v>
       </c>
       <c r="C33">
-        <v>2.385314904566443</v>
+        <v>1.920882962377887</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -6952,10 +6952,10 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>2.271488631347457</v>
+        <v>1.900000000000007</v>
       </c>
       <c r="C35">
-        <v>1.993002426932445</v>
+        <v>1.800000000000009</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -6974,10 +6974,10 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>2.337093805030748</v>
+        <v>1.900000000000059</v>
       </c>
       <c r="C37">
-        <v>2.337093805030748</v>
+        <v>1.800000000000066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>